<commit_message>
fixed game starttime issue
</commit_message>
<xml_diff>
--- a/assets/JCPL 3 Schedule V3 (1).xlsx
+++ b/assets/JCPL 3 Schedule V3 (1).xlsx
@@ -34,10 +34,40 @@
     <t xml:space="preserve">Team 1</t>
   </si>
   <si>
-    <t xml:space="preserve">8th January</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02:40PM – 03PM</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> January</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">03:30PM – 04PM</t>
   </si>
   <si>
     <t xml:space="preserve">Mens</t>
@@ -209,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -231,6 +261,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -447,7 +485,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,8 +569,8 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4068" ySplit="0" topLeftCell="D1" activePane="topLeft" state="split"/>
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <pane xSplit="3948" ySplit="0" topLeftCell="D1" activePane="topLeft" state="split"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>